<commit_message>
update CSR import files
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3example.xlsx
+++ b/curator_data/examples/T3/CSRinT3example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1800" windowWidth="27380" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="1340" windowWidth="27380" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Parameter</t>
   </si>
@@ -84,15 +84,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>By plot -- Will go in raw file</t>
-  </si>
-  <si>
-    <t>Data from weather station?</t>
-  </si>
-  <si>
-    <t>Existing trial annotations</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -135,61 +126,52 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Longitude</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Latitude</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>The following information can be entered in the form. Information with a green background is required, others are optional.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>use Excel date format (ex.  12/5/2011), i.e. with slashes, no leading zeros, and in the month/day/year format.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>Plot size (m</t>
+      <t xml:space="preserve">Use Excel "Text", not "Date", format. The value should be given as </t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <i/>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>2</t>
+      <t>m/d/yyyy</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>)</t>
+      <t xml:space="preserve"> with no leading zeros, e.g. "5/7/2012".</t>
     </r>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5/7/2012</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -224,12 +206,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
@@ -240,13 +216,17 @@
       <family val="2"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
+      <i/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +237,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="49"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,11 +260,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -291,20 +276,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -638,14 +624,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="65.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="106.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -653,122 +641,110 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>40</v>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>25</v>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <v>41199</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>41</v>
+      <c r="B4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>26</v>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>0.54236111111111118</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>0.58402777777777781</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6">
         <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>42</v>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>14</v>
       </c>
     </row>
@@ -776,109 +752,78 @@
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>31</v>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="7">
+        <v>30</v>
+      </c>
+      <c r="B16" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="7">
-        <v>100</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="7">
-        <v>42.944000000000003</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="7">
-        <v>112.837</v>
-      </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>37</v>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
update example templates for CSR
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3example.xlsx
+++ b/curator_data/examples/T3/CSRinT3example.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1340" windowWidth="27380" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="7160" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -36,36 +36,9 @@
     <t>Growth Stage</t>
   </si>
   <si>
-    <t>start time</t>
-  </si>
-  <si>
-    <t>end time</t>
-  </si>
-  <si>
     <t>weather (standardized to clear, hazy, cloudy)</t>
   </si>
   <si>
-    <t>Instrument [JAZ, CropScan]</t>
-  </si>
-  <si>
-    <t>Instrument Detail:</t>
-  </si>
-  <si>
-    <t>Spectrometer serial number</t>
-  </si>
-  <si>
-    <t>Grating Number (e.g., 14 or 3)</t>
-  </si>
-  <si>
-    <t>Collection lens</t>
-  </si>
-  <si>
-    <t>Longpass filter</t>
-  </si>
-  <si>
-    <t>Fiber optic cable type</t>
-  </si>
-  <si>
     <t>Number of measurements per average</t>
   </si>
   <si>
@@ -81,12 +54,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Upwelling</t>
   </si>
   <si>
@@ -99,24 +66,6 @@
     <t>clear</t>
   </si>
   <si>
-    <t>JAZ</t>
-  </si>
-  <si>
-    <t>1k3k3BAZ</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>OFLV</t>
-  </si>
-  <si>
-    <t>Entrance slit aperture (um)</t>
-  </si>
-  <si>
-    <t>P50-2-UV</t>
-  </si>
-  <si>
     <t>barium sulfate</t>
   </si>
   <si>
@@ -127,10 +76,6 @@
   </si>
   <si>
     <t>The following information can be entered in the form. Information with a green background is required, others are optional.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -161,19 +106,45 @@
     <t>5/7/2012</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>This will be ignored if the integration time is included in the raw data file</t>
+  </si>
+  <si>
+    <t>whole day, start time (24-hour clock)</t>
+  </si>
+  <si>
+    <t>whole day, end time (24-hour clock)</t>
+  </si>
+  <si>
+    <t>This will be ignored if the time is included in the raw data file</t>
+  </si>
+  <si>
+    <t>Spectrometer System</t>
+  </si>
+  <si>
+    <t>UCD_WUEoptimzed_Channel1</t>
+  </si>
+  <si>
+    <t>This entry is defined in the "System Name" of the "CSR Spectrometer System"</t>
+  </si>
+  <si>
+    <t>This entry is defined in "Trial Name" of the "Phenotype Experiment"</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>CAP-2_2012_Aberdeen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -224,6 +195,11 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -260,14 +236,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -282,14 +255,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -298,7 +271,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -623,17 +596,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="65.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="50.5" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="106.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,191 +614,149 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>35</v>
+      <c r="B1" s="3"/>
+      <c r="D1" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>21</v>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>37</v>
+      <c r="B4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6">
         <v>0.54236111111111118</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
         <v>0.58402777777777781</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="6">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
         <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>36</v>
+      <c r="D10" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
         <v>10</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="6">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>